<commit_message>
Updated code for test case status reporting. Updated login method
</commit_message>
<xml_diff>
--- a/CertificationProject-HybridFramework/framework/Certification Project Checklist.xlsx
+++ b/CertificationProject-HybridFramework/framework/Certification Project Checklist.xlsx
@@ -10,7 +10,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -693,12 +692,12 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="97.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="97.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -755,7 +754,7 @@
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="10"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6">

</xml_diff>

<commit_message>
Added code for new user registration
</commit_message>
<xml_diff>
--- a/CertificationProject-HybridFramework/framework/Certification Project Checklist.xlsx
+++ b/CertificationProject-HybridFramework/framework/Certification Project Checklist.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18405" windowHeight="7935"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve">Launch http://demo.opensourcecms.com/wordpress/wp-login.php </t>
   </si>
@@ -95,6 +96,9 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>http://newtours.demoaut.com/</t>
   </si>
 </sst>
 </file>
@@ -689,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,6 +931,11 @@
       </c>
       <c r="C25" s="11"/>
     </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>